<commit_message>
adjust template + fix wrong numbers
</commit_message>
<xml_diff>
--- a/Documents/Templates/BrentOfferteTemplate.xlsx
+++ b/Documents/Templates/BrentOfferteTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tvercauteren\Documents\Git\BrentAdmin\Documents\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tvercauteren\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9893749-0255-4C58-8244-48D38A95556A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D570EC-611A-4208-B08F-6874043EF625}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22080" yWindow="792" windowWidth="21600" windowHeight="11388" tabRatio="599" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="599" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="offerte" sheetId="35" r:id="rId1"/>
@@ -564,9 +564,6 @@
     <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -667,6 +664,9 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1160,7 +1160,7 @@
   <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView showGridLines="0" showZeros="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1218,7 +1218,7 @@
       <c r="C6" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="D6" s="66" t="s">
         <v>27</v>
       </c>
       <c r="E6" s="10"/>
@@ -1239,7 +1239,7 @@
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
-      <c r="C9" s="41" t="s">
+      <c r="C9" s="40" t="s">
         <v>41</v>
       </c>
       <c r="D9" s="9" t="s">
@@ -1249,10 +1249,10 @@
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
-      <c r="C10" s="41" t="s">
+      <c r="C10" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="40" t="s">
+      <c r="D10" s="39" t="s">
         <v>29</v>
       </c>
       <c r="E10" s="8"/>
@@ -1271,7 +1271,7 @@
       <c r="A12" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="41" t="s">
+      <c r="C12" s="40" t="s">
         <v>43</v>
       </c>
       <c r="D12" s="9" t="s">
@@ -1283,7 +1283,7 @@
       <c r="A13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="41" t="s">
+      <c r="C13" s="40" t="s">
         <v>44</v>
       </c>
       <c r="D13" s="9" t="s">
@@ -1295,10 +1295,10 @@
       <c r="A14" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="41" t="s">
+      <c r="C14" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="45" t="s">
+      <c r="D14" s="44" t="s">
         <v>32</v>
       </c>
       <c r="E14" s="8"/>
@@ -1307,10 +1307,10 @@
       <c r="A15" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="41" t="s">
+      <c r="C15" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="45" t="s">
+      <c r="D15" s="44" t="s">
         <v>33</v>
       </c>
       <c r="E15" s="8"/>
@@ -1332,11 +1332,11 @@
       <c r="E17" s="8"/>
     </row>
     <row r="18" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="46" t="s">
+      <c r="A18" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="47"/>
-      <c r="C18" s="48"/>
+      <c r="B18" s="46"/>
+      <c r="C18" s="47"/>
       <c r="D18" s="20" t="s">
         <v>1</v>
       </c>
@@ -1350,85 +1350,85 @@
       <c r="E19" s="11"/>
     </row>
     <row r="20" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="49"/>
-      <c r="B20" s="50"/>
-      <c r="C20" s="51"/>
+      <c r="A20" s="48"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="50"/>
       <c r="D20" s="12">
         <v>0</v>
       </c>
       <c r="E20" s="11"/>
     </row>
     <row r="21" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" collapsed="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="64"/>
-      <c r="B21" s="65"/>
-      <c r="C21" s="66"/>
-      <c r="D21" s="28"/>
+      <c r="A21" s="63"/>
+      <c r="B21" s="64"/>
+      <c r="C21" s="65"/>
+      <c r="D21" s="27"/>
       <c r="E21" s="11"/>
     </row>
     <row r="22" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="61" t="s">
+      <c r="A22" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="62"/>
-      <c r="C22" s="63"/>
+      <c r="B22" s="61"/>
+      <c r="C22" s="62"/>
       <c r="D22" s="18"/>
       <c r="E22" s="11"/>
     </row>
     <row r="23" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="42"/>
-      <c r="B23" s="43"/>
-      <c r="C23" s="43"/>
+      <c r="A23" s="41"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="42"/>
       <c r="D23" s="18"/>
       <c r="E23" s="11"/>
     </row>
     <row r="24" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="42" t="s">
+      <c r="A24" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="43"/>
-      <c r="C24" s="43"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="42"/>
       <c r="D24" s="18"/>
       <c r="E24" s="11"/>
     </row>
     <row r="25" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="42"/>
-      <c r="B25" s="43"/>
-      <c r="C25" s="43"/>
+      <c r="A25" s="41"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="42"/>
       <c r="D25" s="18"/>
       <c r="E25" s="11"/>
     </row>
     <row r="26" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="42"/>
-      <c r="B26" s="43"/>
-      <c r="C26" s="43"/>
+      <c r="A26" s="41"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
       <c r="D26" s="18"/>
       <c r="E26" s="11"/>
     </row>
     <row r="27" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="42"/>
-      <c r="B27" s="43"/>
-      <c r="C27" s="43"/>
+      <c r="A27" s="41"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
       <c r="D27" s="18"/>
       <c r="E27" s="11"/>
     </row>
     <row r="28" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="42"/>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
+      <c r="A28" s="41"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="42"/>
       <c r="D28" s="18"/>
-      <c r="E28" s="30"/>
+      <c r="E28" s="29"/>
     </row>
     <row r="29" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="42"/>
-      <c r="B29" s="43"/>
-      <c r="C29" s="43"/>
+      <c r="A29" s="41"/>
+      <c r="B29" s="42"/>
+      <c r="C29" s="42"/>
       <c r="D29" s="18"/>
       <c r="E29" s="11"/>
     </row>
     <row r="30" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="42"/>
-      <c r="B30" s="43"/>
-      <c r="C30" s="44"/>
+      <c r="A30" s="41"/>
+      <c r="B30" s="42"/>
+      <c r="C30" s="43"/>
       <c r="D30" s="12"/>
       <c r="E30" s="11"/>
     </row>
@@ -1451,33 +1451,33 @@
       <c r="E32" s="11"/>
     </row>
     <row r="33" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="52" t="s">
+      <c r="A33" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="B33" s="53"/>
-      <c r="C33" s="54"/>
-      <c r="D33" s="31" t="s">
+      <c r="B33" s="52"/>
+      <c r="C33" s="53"/>
+      <c r="D33" s="30" t="s">
         <v>34</v>
       </c>
       <c r="E33" s="11"/>
     </row>
     <row r="34" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="55" t="s">
+      <c r="A34" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="B34" s="56"/>
-      <c r="C34" s="57"/>
+      <c r="B34" s="55"/>
+      <c r="C34" s="56"/>
       <c r="D34" s="12" t="s">
         <v>35</v>
       </c>
       <c r="E34" s="11"/>
     </row>
     <row r="35" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="58" t="s">
+      <c r="A35" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="B35" s="59"/>
-      <c r="C35" s="60"/>
+      <c r="B35" s="58"/>
+      <c r="C35" s="59"/>
       <c r="D35" s="13" t="s">
         <v>36</v>
       </c>
@@ -1515,7 +1515,7 @@
         <v>24</v>
       </c>
       <c r="B39" s="6"/>
-      <c r="D39" s="39" t="s">
+      <c r="D39" s="38" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1524,7 +1524,7 @@
         <v>23</v>
       </c>
       <c r="B40" s="6"/>
-      <c r="D40" s="39" t="s">
+      <c r="D40" s="38" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1547,79 +1547,79 @@
       <c r="B44" s="6"/>
     </row>
     <row r="45" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A45" s="32" t="s">
+      <c r="A45" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="B45" s="33"/>
+      <c r="B45" s="32"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="34"/>
-      <c r="B46" s="35"/>
+      <c r="A46" s="33"/>
+      <c r="B46" s="34"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="34"/>
-      <c r="B47" s="35"/>
+      <c r="A47" s="33"/>
+      <c r="B47" s="34"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="34"/>
-      <c r="B48" s="35"/>
+      <c r="A48" s="33"/>
+      <c r="B48" s="34"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="34"/>
-      <c r="B49" s="35"/>
+      <c r="A49" s="33"/>
+      <c r="B49" s="34"/>
     </row>
     <row r="50" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A50" s="36"/>
-      <c r="B50" s="35"/>
+      <c r="A50" s="35"/>
+      <c r="B50" s="34"/>
     </row>
     <row r="51" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="37" t="s">
+      <c r="A51" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="B51" s="38" t="s">
+      <c r="B51" s="37" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A52" s="29"/>
+      <c r="A52" s="28"/>
       <c r="B52" s="6"/>
     </row>
     <row r="53" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A53" s="29"/>
+      <c r="A53" s="28"/>
       <c r="B53" s="6"/>
     </row>
     <row r="54" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A54" s="29" t="s">
+      <c r="A54" s="28" t="s">
         <v>16</v>
       </c>
       <c r="B54" s="6"/>
     </row>
     <row r="55" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A55" s="29"/>
+      <c r="A55" s="28"/>
       <c r="B55" s="6"/>
     </row>
     <row r="56" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A56" s="29"/>
+      <c r="A56" s="28"/>
       <c r="B56" s="6"/>
     </row>
     <row r="57" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A57" s="29"/>
+      <c r="A57" s="28"/>
       <c r="B57" s="6"/>
     </row>
     <row r="58" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A58" s="29"/>
+      <c r="A58" s="28"/>
       <c r="B58" s="6"/>
     </row>
     <row r="59" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A59" s="29"/>
+      <c r="A59" s="28"/>
       <c r="B59" s="6"/>
     </row>
     <row r="60" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A60" s="29"/>
+      <c r="A60" s="28"/>
       <c r="B60" s="6"/>
     </row>
     <row r="61" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A61" s="29"/>
+      <c r="A61" s="28"/>
       <c r="B61" s="6"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
revert to excel usage + voorschot aanpassingen
</commit_message>
<xml_diff>
--- a/Documents/Templates/BrentOfferteTemplate.xlsx
+++ b/Documents/Templates/BrentOfferteTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tvercauteren\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D570EC-611A-4208-B08F-6874043EF625}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EDCCD05-332C-481D-BF52-7E2E0BA37986}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="599" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>OMSCHRIJVING</t>
   </si>
@@ -52,9 +52,6 @@
     <t>VERVALDATUM</t>
   </si>
   <si>
-    <t>Offerte</t>
-  </si>
-  <si>
     <t>BTW 6%</t>
   </si>
   <si>
@@ -154,9 +151,6 @@
     <t>{{PrijsLeftOver}}</t>
   </si>
   <si>
-    <t>{{items.Description}}</t>
-  </si>
-  <si>
     <t>Klant :</t>
   </si>
   <si>
@@ -188,16 +182,60 @@
   </si>
   <si>
     <t>Medecontractant</t>
+  </si>
+  <si>
+    <t>{{Type}}</t>
+  </si>
+  <si>
+    <t>{{Item1}}</t>
+  </si>
+  <si>
+    <t>{{Item1Prijs}}</t>
+  </si>
+  <si>
+    <t>{{Item2Prijs}}</t>
+  </si>
+  <si>
+    <t>{{Item3Prijs}}</t>
+  </si>
+  <si>
+    <t>{{Item4Prijs}}</t>
+  </si>
+  <si>
+    <t>{{Item5Prijs}}</t>
+  </si>
+  <si>
+    <t>{{Item6Prijs}}</t>
+  </si>
+  <si>
+    <t>{{FactuurItemPrijs}}</t>
+  </si>
+  <si>
+    <t>{{Item2}}</t>
+  </si>
+  <si>
+    <t>{{Item3}}</t>
+  </si>
+  <si>
+    <t>{{Item4}}</t>
+  </si>
+  <si>
+    <t>{{Item5}}</t>
+  </si>
+  <si>
+    <t>{{Item6}}</t>
+  </si>
+  <si>
+    <t>{{FactuurItem}}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_-&quot;€&quot;\ * #,##0.00_-;\-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * #,##0.00\-;_-&quot;€&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="@\ \ "/>
     <numFmt numFmtId="167" formatCode="[$-413]d\ mmmm\ yyyy;@"/>
   </numFmts>
@@ -496,7 +534,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -526,9 +564,6 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -541,17 +576,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -564,15 +593,9 @@
     <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -583,7 +606,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -665,7 +687,32 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -764,21 +811,21 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1356360</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>2476499</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>184352</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1155" name="Afbeelding 4">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000083040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FCFAF7B7-B667-439E-BA8A-866FE6FFC4EF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -789,42 +836,18 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect l="10440" t="13005" r="15063" b="66414"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="4587240" cy="1983105"/>
+          <a:ext cx="5705474" cy="1898852"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1159,8 +1182,8 @@
   </sheetPr>
   <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1175,8 +1198,8 @@
     <row r="1" spans="1:5" ht="42.75" x14ac:dyDescent="0.8">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="D1" s="19" t="s">
-        <v>6</v>
+      <c r="D1" s="17" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
@@ -1195,31 +1218,31 @@
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="26" t="s">
-        <v>25</v>
+      <c r="D4" s="23" t="s">
+        <v>24</v>
       </c>
       <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="26" t="s">
-        <v>26</v>
+      <c r="D5" s="23" t="s">
+        <v>25</v>
       </c>
       <c r="E5" s="8"/>
     </row>
     <row r="6" spans="1:5" s="5" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
-      <c r="C6" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="66" t="s">
-        <v>27</v>
+      <c r="C6" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="69" t="s">
+        <v>26</v>
       </c>
       <c r="E6" s="10"/>
     </row>
@@ -1239,31 +1262,31 @@
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
-      <c r="C9" s="40" t="s">
-        <v>41</v>
+      <c r="C9" s="34" t="s">
+        <v>39</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
-      <c r="C10" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="39" t="s">
-        <v>29</v>
+      <c r="C10" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>28</v>
       </c>
       <c r="E10" s="8"/>
     </row>
     <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E11" s="8"/>
     </row>
@@ -1271,53 +1294,53 @@
       <c r="A12" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>30</v>
+      <c r="C12" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="68" t="s">
+        <v>29</v>
       </c>
       <c r="E12" s="8"/>
     </row>
     <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>31</v>
+        <v>12</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="68" t="s">
+        <v>30</v>
       </c>
       <c r="E13" s="8"/>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="44" t="s">
-        <v>32</v>
+        <v>46</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="38" t="s">
+        <v>31</v>
       </c>
       <c r="E14" s="8"/>
     </row>
     <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" s="44" t="s">
-        <v>33</v>
+        <v>45</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="68" t="s">
+        <v>32</v>
       </c>
       <c r="E15" s="8"/>
     </row>
     <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -1332,12 +1355,12 @@
       <c r="E17" s="8"/>
     </row>
     <row r="18" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="45" t="s">
+      <c r="A18" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="46"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="20" t="s">
+      <c r="B18" s="40"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="18" t="s">
         <v>1</v>
       </c>
       <c r="E18" s="11"/>
@@ -1350,147 +1373,173 @@
       <c r="E19" s="11"/>
     </row>
     <row r="20" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="48"/>
-      <c r="B20" s="49"/>
-      <c r="C20" s="50"/>
+      <c r="A20" s="42"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="44"/>
       <c r="D20" s="12">
         <v>0</v>
       </c>
       <c r="E20" s="11"/>
     </row>
     <row r="21" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" collapsed="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="63"/>
-      <c r="B21" s="64"/>
-      <c r="C21" s="65"/>
-      <c r="D21" s="27"/>
+      <c r="A21" s="57"/>
+      <c r="B21" s="58"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="63"/>
       <c r="E21" s="11"/>
     </row>
     <row r="22" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="60" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="61"/>
-      <c r="C22" s="62"/>
-      <c r="D22" s="18"/>
+      <c r="A22" s="54" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="55"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="64"/>
       <c r="E22" s="11"/>
     </row>
     <row r="23" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="41"/>
-      <c r="B23" s="42"/>
-      <c r="C23" s="42"/>
-      <c r="D23" s="18"/>
+      <c r="A23" s="35"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="64"/>
       <c r="E23" s="11"/>
     </row>
     <row r="24" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="B24" s="42"/>
-      <c r="C24" s="42"/>
-      <c r="D24" s="18"/>
+      <c r="A24" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="36"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="60" t="s">
+        <v>52</v>
+      </c>
       <c r="E24" s="11"/>
     </row>
     <row r="25" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="41"/>
-      <c r="B25" s="42"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="18"/>
+      <c r="A25" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="36"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="60" t="s">
+        <v>53</v>
+      </c>
       <c r="E25" s="11"/>
     </row>
     <row r="26" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="41"/>
-      <c r="B26" s="42"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="18"/>
+      <c r="A26" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="36"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="60" t="s">
+        <v>54</v>
+      </c>
       <c r="E26" s="11"/>
     </row>
     <row r="27" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="41"/>
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="18"/>
+      <c r="A27" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="60" t="s">
+        <v>55</v>
+      </c>
       <c r="E27" s="11"/>
     </row>
     <row r="28" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="41"/>
-      <c r="B28" s="42"/>
-      <c r="C28" s="42"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="29"/>
+      <c r="A28" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="60" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28" s="25"/>
     </row>
     <row r="29" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="41"/>
-      <c r="B29" s="42"/>
-      <c r="C29" s="42"/>
-      <c r="D29" s="18"/>
+      <c r="A29" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" s="36"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="60" t="s">
+        <v>57</v>
+      </c>
       <c r="E29" s="11"/>
     </row>
     <row r="30" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="41"/>
-      <c r="B30" s="42"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="12"/>
+      <c r="A30" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" s="36"/>
+      <c r="C30" s="37"/>
+      <c r="D30" s="60" t="s">
+        <v>58</v>
+      </c>
       <c r="E30" s="11"/>
     </row>
     <row r="31" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="23" t="s">
+      <c r="A31" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="13"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="61" t="s">
+        <v>48</v>
+      </c>
+      <c r="E31" s="11"/>
+    </row>
+    <row r="32" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="15"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="61"/>
+      <c r="E32" s="11"/>
+    </row>
+    <row r="33" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="46"/>
+      <c r="C33" s="47"/>
+      <c r="D33" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="E33" s="11"/>
+    </row>
+    <row r="34" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="14"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="E31" s="11"/>
-    </row>
-    <row r="32" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="16"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="11"/>
-    </row>
-    <row r="33" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="B33" s="52"/>
-      <c r="C33" s="53"/>
-      <c r="D33" s="30" t="s">
+      <c r="B34" s="49"/>
+      <c r="C34" s="50"/>
+      <c r="D34" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="E33" s="11"/>
-    </row>
-    <row r="34" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="54" t="s">
-        <v>10</v>
-      </c>
-      <c r="B34" s="55"/>
-      <c r="C34" s="56"/>
-      <c r="D34" s="12" t="s">
+      <c r="E34" s="11"/>
+    </row>
+    <row r="35" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35" s="52"/>
+      <c r="C35" s="53"/>
+      <c r="D35" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="E34" s="11"/>
-    </row>
-    <row r="35" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="57" t="s">
-        <v>51</v>
-      </c>
-      <c r="B35" s="58"/>
-      <c r="C35" s="59"/>
-      <c r="D35" s="13" t="s">
+      <c r="E35" s="11"/>
+    </row>
+    <row r="36" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="13"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36" s="65" t="s">
         <v>36</v>
-      </c>
-      <c r="E35" s="11"/>
-    </row>
-    <row r="36" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="14"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="D36" s="21" t="s">
-        <v>37</v>
       </c>
       <c r="E36" s="11"/>
     </row>
@@ -1498,38 +1547,38 @@
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
+      <c r="D37" s="66"/>
       <c r="E37" s="8"/>
     </row>
     <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="22" t="s">
-        <v>11</v>
+      <c r="A38" s="19" t="s">
+        <v>10</v>
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
+      <c r="D38" s="66"/>
       <c r="E38" s="8"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="24" t="s">
-        <v>24</v>
+      <c r="A39" s="21" t="s">
+        <v>23</v>
       </c>
       <c r="B39" s="6"/>
-      <c r="D39" s="38" t="s">
+      <c r="D39" s="67" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B40" s="6"/>
+      <c r="D40" s="67" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="B40" s="6"/>
-      <c r="D40" s="38" t="s">
-        <v>39</v>
-      </c>
-    </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="24"/>
+      <c r="A41" s="21"/>
       <c r="B41" s="6"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -1537,8 +1586,8 @@
       <c r="B42" s="6"/>
     </row>
     <row r="43" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="22" t="s">
-        <v>18</v>
+      <c r="A43" s="19" t="s">
+        <v>17</v>
       </c>
       <c r="B43" s="6"/>
     </row>
@@ -1547,79 +1596,79 @@
       <c r="B44" s="6"/>
     </row>
     <row r="45" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A45" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="B45" s="32"/>
+      <c r="A45" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B45" s="27"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="33"/>
-      <c r="B46" s="34"/>
+      <c r="A46" s="28"/>
+      <c r="B46" s="29"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="33"/>
-      <c r="B47" s="34"/>
+      <c r="A47" s="28"/>
+      <c r="B47" s="29"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="33"/>
-      <c r="B48" s="34"/>
+      <c r="A48" s="28"/>
+      <c r="B48" s="29"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="33"/>
-      <c r="B49" s="34"/>
+      <c r="A49" s="28"/>
+      <c r="B49" s="29"/>
     </row>
     <row r="50" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A50" s="35"/>
-      <c r="B50" s="34"/>
+      <c r="A50" s="30"/>
+      <c r="B50" s="29"/>
     </row>
     <row r="51" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="36" t="s">
+      <c r="A51" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B51" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B51" s="37" t="s">
+    </row>
+    <row r="52" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A52" s="24"/>
+      <c r="B52" s="6"/>
+    </row>
+    <row r="53" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A53" s="24"/>
+      <c r="B53" s="6"/>
+    </row>
+    <row r="54" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A54" s="24" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A52" s="28"/>
-      <c r="B52" s="6"/>
-    </row>
-    <row r="53" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A53" s="28"/>
-      <c r="B53" s="6"/>
-    </row>
-    <row r="54" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A54" s="28" t="s">
-        <v>16</v>
-      </c>
       <c r="B54" s="6"/>
     </row>
     <row r="55" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A55" s="28"/>
+      <c r="A55" s="24"/>
       <c r="B55" s="6"/>
     </row>
     <row r="56" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A56" s="28"/>
+      <c r="A56" s="24"/>
       <c r="B56" s="6"/>
     </row>
     <row r="57" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A57" s="28"/>
+      <c r="A57" s="24"/>
       <c r="B57" s="6"/>
     </row>
     <row r="58" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A58" s="28"/>
+      <c r="A58" s="24"/>
       <c r="B58" s="6"/>
     </row>
     <row r="59" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A59" s="28"/>
+      <c r="A59" s="24"/>
       <c r="B59" s="6"/>
     </row>
     <row r="60" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A60" s="28"/>
+      <c r="A60" s="24"/>
       <c r="B60" s="6"/>
     </row>
     <row r="61" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A61" s="28"/>
+      <c r="A61" s="24"/>
       <c r="B61" s="6"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
@@ -1628,13 +1677,13 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B63" s="6"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B64" s="6"/>
     </row>
@@ -1655,13 +1704,9 @@
     <mergeCell ref="A21:C21"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="A16" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D15" r:id="rId2" display="mainil.eveline@gmail.com" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-  </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" scale="62" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup paperSize="9" scale="68" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId4"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add changes to factuurnummer
</commit_message>
<xml_diff>
--- a/Documents/Templates/BrentOfferteTemplate.xlsx
+++ b/Documents/Templates/BrentOfferteTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tvercauteren\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\source\repos\BrentAdmin\Documents\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EDCCD05-332C-481D-BF52-7E2E0BA37986}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E9B1F62-B8CF-424F-A60E-38DB6685C05D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="599" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="599" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="offerte" sheetId="35" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>OMSCHRIJVING</t>
   </si>
@@ -169,12 +169,6 @@
     <t>Email:</t>
   </si>
   <si>
-    <t>IBAN: BE58 7360 1926 5779</t>
-  </si>
-  <si>
-    <t>BTW: BE 0636.881.313</t>
-  </si>
-  <si>
     <t>{{KlantPostcodeGemeente}}</t>
   </si>
   <si>
@@ -227,6 +221,15 @@
   </si>
   <si>
     <t>{{FactuurItem}}</t>
+  </si>
+  <si>
+    <t>BTW: BE 0763.510.556</t>
+  </si>
+  <si>
+    <t>IBAN: BE17 7340 4965 5521</t>
+  </si>
+  <si>
+    <t>Brent Wiels Maatwerk BV</t>
   </si>
 </sst>
 </file>
@@ -236,8 +239,8 @@
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-&quot;€&quot;\ * #,##0.00_-;\-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="@\ \ "/>
-    <numFmt numFmtId="167" formatCode="[$-413]d\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="@\ \ "/>
+    <numFmt numFmtId="166" formatCode="[$-413]d\ mmmm\ yyyy;@"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -567,7 +570,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -590,7 +593,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -624,69 +627,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -714,6 +654,69 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1182,41 +1185,41 @@
   </sheetPr>
   <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.42578125" customWidth="1"/>
-    <col min="2" max="2" width="37.140625" customWidth="1"/>
+    <col min="1" max="1" width="48.453125" customWidth="1"/>
+    <col min="2" max="2" width="37.1796875" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.81640625" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="42.75" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:5" ht="43" x14ac:dyDescent="1.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="D1" s="17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="8"/>
       <c r="C4" s="22" t="s">
         <v>2</v>
@@ -1226,7 +1229,7 @@
       </c>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="8"/>
       <c r="C5" s="22" t="s">
         <v>5</v>
@@ -1236,31 +1239,31 @@
       </c>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" spans="1:5" s="5" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="5" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="C6" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="69" t="s">
+      <c r="D6" s="48" t="s">
         <v>26</v>
       </c>
       <c r="E6" s="10"/>
     </row>
-    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
     </row>
-    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="9"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
     </row>
-    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="8"/>
       <c r="C9" s="34" t="s">
         <v>39</v>
@@ -1270,8 +1273,10 @@
       </c>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
+    <row r="10" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="19" t="s">
+        <v>65</v>
+      </c>
       <c r="C10" s="34" t="s">
         <v>40</v>
       </c>
@@ -1280,43 +1285,43 @@
       </c>
       <c r="E10" s="8"/>
     </row>
-    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E11" s="8"/>
     </row>
-    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="68" t="s">
+      <c r="D12" s="47" t="s">
         <v>29</v>
       </c>
       <c r="E12" s="8"/>
     </row>
-    <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="68" t="s">
+      <c r="D13" s="47" t="s">
         <v>30</v>
       </c>
       <c r="E13" s="8"/>
     </row>
-    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="C14" s="34" t="s">
         <v>43</v>
@@ -1326,19 +1331,19 @@
       </c>
       <c r="E14" s="8"/>
     </row>
-    <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="C15" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="68" t="s">
+      <c r="D15" s="47" t="s">
         <v>32</v>
       </c>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
         <v>11</v>
       </c>
@@ -1347,281 +1352,281 @@
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
     </row>
-    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
     </row>
-    <row r="18" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="39" t="s">
+    <row r="18" spans="1:5" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="40"/>
-      <c r="C18" s="41"/>
+      <c r="B18" s="50"/>
+      <c r="C18" s="51"/>
       <c r="D18" s="18" t="s">
         <v>1</v>
       </c>
       <c r="E18" s="11"/>
     </row>
-    <row r="19" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
     </row>
-    <row r="20" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="42"/>
-      <c r="B20" s="43"/>
-      <c r="C20" s="44"/>
+    <row r="20" spans="1:5" s="2" customFormat="1" ht="20.149999999999999" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="52"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="54"/>
       <c r="D20" s="12">
         <v>0</v>
       </c>
       <c r="E20" s="11"/>
     </row>
-    <row r="21" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" collapsed="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="57"/>
-      <c r="B21" s="58"/>
-      <c r="C21" s="59"/>
-      <c r="D21" s="63"/>
+    <row r="21" spans="1:5" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="67"/>
+      <c r="B21" s="68"/>
+      <c r="C21" s="69"/>
+      <c r="D21" s="42"/>
       <c r="E21" s="11"/>
     </row>
-    <row r="22" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="54" t="s">
+    <row r="22" spans="1:5" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="55"/>
-      <c r="C22" s="56"/>
-      <c r="D22" s="64"/>
+      <c r="B22" s="65"/>
+      <c r="C22" s="66"/>
+      <c r="D22" s="43"/>
       <c r="E22" s="11"/>
     </row>
-    <row r="23" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="35"/>
       <c r="B23" s="36"/>
       <c r="C23" s="36"/>
-      <c r="D23" s="64"/>
+      <c r="D23" s="43"/>
       <c r="E23" s="11"/>
     </row>
-    <row r="24" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="35" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B24" s="36"/>
       <c r="C24" s="36"/>
-      <c r="D24" s="60" t="s">
-        <v>52</v>
+      <c r="D24" s="39" t="s">
+        <v>50</v>
       </c>
       <c r="E24" s="11"/>
     </row>
-    <row r="25" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="35" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B25" s="36"/>
       <c r="C25" s="36"/>
-      <c r="D25" s="60" t="s">
-        <v>53</v>
+      <c r="D25" s="39" t="s">
+        <v>51</v>
       </c>
       <c r="E25" s="11"/>
     </row>
-    <row r="26" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="35" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B26" s="36"/>
       <c r="C26" s="36"/>
-      <c r="D26" s="60" t="s">
-        <v>54</v>
+      <c r="D26" s="39" t="s">
+        <v>52</v>
       </c>
       <c r="E26" s="11"/>
     </row>
-    <row r="27" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="35" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B27" s="36"/>
       <c r="C27" s="36"/>
-      <c r="D27" s="60" t="s">
-        <v>55</v>
+      <c r="D27" s="39" t="s">
+        <v>53</v>
       </c>
       <c r="E27" s="11"/>
     </row>
-    <row r="28" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="35" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B28" s="36"/>
       <c r="C28" s="36"/>
-      <c r="D28" s="60" t="s">
-        <v>56</v>
+      <c r="D28" s="39" t="s">
+        <v>54</v>
       </c>
       <c r="E28" s="25"/>
     </row>
-    <row r="29" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="35" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B29" s="36"/>
       <c r="C29" s="36"/>
-      <c r="D29" s="60" t="s">
-        <v>57</v>
+      <c r="D29" s="39" t="s">
+        <v>55</v>
       </c>
       <c r="E29" s="11"/>
     </row>
-    <row r="30" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="35" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B30" s="36"/>
       <c r="C30" s="37"/>
-      <c r="D30" s="60" t="s">
-        <v>58</v>
+      <c r="D30" s="39" t="s">
+        <v>56</v>
       </c>
       <c r="E30" s="11"/>
     </row>
-    <row r="31" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>8</v>
       </c>
       <c r="B31" s="13"/>
       <c r="C31" s="16"/>
-      <c r="D31" s="61" t="s">
-        <v>48</v>
+      <c r="D31" s="40" t="s">
+        <v>46</v>
       </c>
       <c r="E31" s="11"/>
     </row>
-    <row r="32" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="15"/>
       <c r="B32" s="13"/>
       <c r="C32" s="16"/>
-      <c r="D32" s="61"/>
+      <c r="D32" s="40"/>
       <c r="E32" s="11"/>
     </row>
-    <row r="33" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="45" t="s">
+    <row r="33" spans="1:5" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="B33" s="46"/>
-      <c r="C33" s="47"/>
-      <c r="D33" s="61" t="s">
+      <c r="B33" s="56"/>
+      <c r="C33" s="57"/>
+      <c r="D33" s="40" t="s">
         <v>33</v>
       </c>
       <c r="E33" s="11"/>
     </row>
-    <row r="34" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="48" t="s">
+    <row r="34" spans="1:5" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="49"/>
-      <c r="C34" s="50"/>
-      <c r="D34" s="61" t="s">
+      <c r="B34" s="59"/>
+      <c r="C34" s="60"/>
+      <c r="D34" s="40" t="s">
         <v>34</v>
       </c>
       <c r="E34" s="11"/>
     </row>
-    <row r="35" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="B35" s="52"/>
-      <c r="C35" s="53"/>
-      <c r="D35" s="62" t="s">
+    <row r="35" spans="1:5" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="61" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" s="62"/>
+      <c r="C35" s="63"/>
+      <c r="D35" s="41" t="s">
         <v>35</v>
       </c>
       <c r="E35" s="11"/>
     </row>
-    <row r="36" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
       <c r="B36" s="13"/>
       <c r="C36" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D36" s="65" t="s">
+      <c r="D36" s="44" t="s">
         <v>36</v>
       </c>
       <c r="E36" s="11"/>
     </row>
-    <row r="37" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
-      <c r="D37" s="66"/>
+      <c r="D37" s="45"/>
       <c r="E37" s="8"/>
     </row>
-    <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A38" s="19" t="s">
         <v>10</v>
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
-      <c r="D38" s="66"/>
+      <c r="D38" s="45"/>
       <c r="E38" s="8"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="21" t="s">
         <v>23</v>
       </c>
       <c r="B39" s="6"/>
-      <c r="D39" s="67" t="s">
+      <c r="D39" s="46" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="21" t="s">
         <v>22</v>
       </c>
       <c r="B40" s="6"/>
-      <c r="D40" s="67" t="s">
+      <c r="D40" s="46" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="21"/>
       <c r="B41" s="6"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
     </row>
-    <row r="43" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A43" s="19" t="s">
         <v>17</v>
       </c>
       <c r="B43" s="6"/>
     </row>
-    <row r="44" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="6"/>
       <c r="B44" s="6"/>
     </row>
-    <row r="45" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A45" s="26" t="s">
         <v>19</v>
       </c>
       <c r="B45" s="27"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="28"/>
       <c r="B46" s="29"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="28"/>
       <c r="B47" s="29"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="28"/>
       <c r="B48" s="29"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="28"/>
       <c r="B49" s="29"/>
     </row>
-    <row r="50" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A50" s="30"/>
       <c r="B50" s="29"/>
     </row>
-    <row r="51" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="31" t="s">
         <v>13</v>
       </c>
@@ -1629,65 +1634,65 @@
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A52" s="24"/>
       <c r="B52" s="6"/>
     </row>
-    <row r="53" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A53" s="24"/>
       <c r="B53" s="6"/>
     </row>
-    <row r="54" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A54" s="24" t="s">
         <v>15</v>
       </c>
       <c r="B54" s="6"/>
     </row>
-    <row r="55" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A55" s="24"/>
       <c r="B55" s="6"/>
     </row>
-    <row r="56" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A56" s="24"/>
       <c r="B56" s="6"/>
     </row>
-    <row r="57" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A57" s="24"/>
       <c r="B57" s="6"/>
     </row>
-    <row r="58" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A58" s="24"/>
       <c r="B58" s="6"/>
     </row>
-    <row r="59" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A59" s="24"/>
       <c r="B59" s="6"/>
     </row>
-    <row r="60" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A60" s="24"/>
       <c r="B60" s="6"/>
     </row>
-    <row r="61" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A61" s="24"/>
       <c r="B61" s="6"/>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="7"/>
       <c r="B62" s="7"/>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B63" s="6"/>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B64" s="6"/>
     </row>
-    <row r="66" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>

</xml_diff>